<commit_message>
update of new_formulation (still not working)
Aggiornamento new_formulation con insulation e costi operativi su tutto l'anno (ma ancora errore su activities2)
</commit_message>
<xml_diff>
--- a/thesis/main_new_formulation/concept_new_storage.xlsx
+++ b/thesis/main_new_formulation/concept_new_storage.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cami/Documents/GitHub/pyesm_tesi/thesis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cami/Documents/GitHub/pyesm_tesi/thesis/main_new_formulation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AED1F7A-0173-9444-A1A4-3BA97617AFA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{062C9EA9-37B3-0E4F-9BE3-5645AB31248A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1820" yWindow="-17500" windowWidth="32000" windowHeight="17500" xr2:uid="{7B02621E-B7BE-C640-8F0D-21B2A43A72CA}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{7B02621E-B7BE-C640-8F0D-21B2A43A72CA}"/>
   </bookViews>
   <sheets>
     <sheet name="new" sheetId="10" r:id="rId1"/>
@@ -907,8 +907,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1245,14 +1245,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B097AE1A-0E18-DF48-8976-354601D23DDF}">
   <dimension ref="A1:CP74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AW1" workbookViewId="0">
-      <selection activeCell="BQ22" sqref="BQ22"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="75" workbookViewId="0">
+      <selection activeCell="X39" sqref="X39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="7" max="7" width="18.1640625" customWidth="1"/>
     <col min="8" max="8" width="10.83203125" style="31"/>
+    <col min="40" max="40" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:94" x14ac:dyDescent="0.2">
@@ -1719,7 +1720,7 @@
         <v>41</v>
       </c>
       <c r="H7" s="2"/>
-      <c r="I7" s="60"/>
+      <c r="I7" s="1"/>
       <c r="J7" s="6" t="s">
         <v>42</v>
       </c>
@@ -1860,7 +1861,7 @@
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="61" t="s">
+      <c r="H8" s="60" t="s">
         <v>55</v>
       </c>
       <c r="I8" s="8"/>
@@ -2085,46 +2086,46 @@
         <v>56</v>
       </c>
       <c r="I10" s="3"/>
-      <c r="J10" s="12">
-        <v>1</v>
-      </c>
-      <c r="K10" s="12">
-        <v>1</v>
-      </c>
-      <c r="L10" s="12">
-        <v>1</v>
-      </c>
-      <c r="M10" s="12">
-        <v>1</v>
-      </c>
-      <c r="N10" s="12">
-        <v>0</v>
-      </c>
-      <c r="O10" s="12">
-        <v>0</v>
-      </c>
-      <c r="P10" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="12">
-        <v>0</v>
-      </c>
-      <c r="R10" s="12">
-        <v>0</v>
-      </c>
-      <c r="S10" s="12">
-        <v>0</v>
-      </c>
-      <c r="T10" s="12">
-        <v>0</v>
-      </c>
-      <c r="U10" s="12">
-        <v>0</v>
-      </c>
-      <c r="V10" s="12">
-        <v>0</v>
-      </c>
-      <c r="W10" s="12">
+      <c r="J10" s="14">
+        <v>1</v>
+      </c>
+      <c r="K10" s="14">
+        <v>1</v>
+      </c>
+      <c r="L10" s="14">
+        <v>1</v>
+      </c>
+      <c r="M10" s="14">
+        <v>1</v>
+      </c>
+      <c r="N10" s="14">
+        <v>0</v>
+      </c>
+      <c r="O10" s="14">
+        <v>0</v>
+      </c>
+      <c r="P10" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="14">
+        <v>0</v>
+      </c>
+      <c r="R10" s="14">
+        <v>0</v>
+      </c>
+      <c r="S10" s="14">
+        <v>0</v>
+      </c>
+      <c r="T10" s="14">
+        <v>0</v>
+      </c>
+      <c r="U10" s="14">
+        <v>0</v>
+      </c>
+      <c r="V10" s="14">
+        <v>0</v>
+      </c>
+      <c r="W10" s="14">
         <v>0</v>
       </c>
       <c r="X10" s="13"/>
@@ -2311,46 +2312,46 @@
         <v>56</v>
       </c>
       <c r="I11" s="3"/>
-      <c r="J11" s="12">
-        <v>0</v>
-      </c>
-      <c r="K11" s="12">
-        <v>0</v>
-      </c>
-      <c r="L11" s="12">
-        <v>0</v>
-      </c>
-      <c r="M11" s="12">
-        <v>0</v>
-      </c>
-      <c r="N11" s="12">
-        <v>1</v>
-      </c>
-      <c r="O11" s="12">
-        <v>0</v>
-      </c>
-      <c r="P11" s="12">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="12">
-        <v>1</v>
-      </c>
-      <c r="R11" s="12">
-        <v>0</v>
-      </c>
-      <c r="S11" s="12">
-        <v>0</v>
-      </c>
-      <c r="T11" s="12">
-        <v>0</v>
-      </c>
-      <c r="U11" s="12">
-        <v>0</v>
-      </c>
-      <c r="V11" s="12">
-        <v>0</v>
-      </c>
-      <c r="W11" s="12">
+      <c r="J11" s="14">
+        <v>0</v>
+      </c>
+      <c r="K11" s="14">
+        <v>0</v>
+      </c>
+      <c r="L11" s="14">
+        <v>0</v>
+      </c>
+      <c r="M11" s="14">
+        <v>0</v>
+      </c>
+      <c r="N11" s="14">
+        <v>1</v>
+      </c>
+      <c r="O11" s="14">
+        <v>0</v>
+      </c>
+      <c r="P11" s="14">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="14">
+        <v>1</v>
+      </c>
+      <c r="R11" s="14">
+        <v>0</v>
+      </c>
+      <c r="S11" s="14">
+        <v>0</v>
+      </c>
+      <c r="T11" s="14">
+        <v>0</v>
+      </c>
+      <c r="U11" s="14">
+        <v>0</v>
+      </c>
+      <c r="V11" s="14">
+        <v>0</v>
+      </c>
+      <c r="W11" s="14">
         <v>0</v>
       </c>
       <c r="X11" s="13"/>
@@ -2534,46 +2535,46 @@
         <v>56</v>
       </c>
       <c r="I12" s="3"/>
-      <c r="J12" s="12">
-        <v>0</v>
-      </c>
-      <c r="K12" s="12">
-        <v>0</v>
-      </c>
-      <c r="L12" s="12">
-        <v>0</v>
-      </c>
-      <c r="M12" s="12">
-        <v>0</v>
-      </c>
-      <c r="N12" s="12">
-        <v>0</v>
-      </c>
-      <c r="O12" s="12">
-        <v>1</v>
-      </c>
-      <c r="P12" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="12">
-        <v>0</v>
-      </c>
-      <c r="R12" s="12">
-        <v>0</v>
-      </c>
-      <c r="S12" s="12">
-        <v>0</v>
-      </c>
-      <c r="T12" s="12">
-        <v>1</v>
-      </c>
-      <c r="U12" s="12">
-        <v>0</v>
-      </c>
-      <c r="V12" s="12">
-        <v>0</v>
-      </c>
-      <c r="W12" s="12">
+      <c r="J12" s="14">
+        <v>0</v>
+      </c>
+      <c r="K12" s="14">
+        <v>0</v>
+      </c>
+      <c r="L12" s="14">
+        <v>0</v>
+      </c>
+      <c r="M12" s="14">
+        <v>0</v>
+      </c>
+      <c r="N12" s="14">
+        <v>0</v>
+      </c>
+      <c r="O12" s="14">
+        <v>1</v>
+      </c>
+      <c r="P12" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="14">
+        <v>0</v>
+      </c>
+      <c r="R12" s="14">
+        <v>0</v>
+      </c>
+      <c r="S12" s="14">
+        <v>0</v>
+      </c>
+      <c r="T12" s="14">
+        <v>1</v>
+      </c>
+      <c r="U12" s="14">
+        <v>0</v>
+      </c>
+      <c r="V12" s="14">
+        <v>0</v>
+      </c>
+      <c r="W12" s="14">
         <v>0</v>
       </c>
       <c r="X12" s="13"/>
@@ -2742,46 +2743,46 @@
         <v>56</v>
       </c>
       <c r="I13" s="3"/>
-      <c r="J13" s="12">
-        <v>0</v>
-      </c>
-      <c r="K13" s="12">
-        <v>0</v>
-      </c>
-      <c r="L13" s="12">
-        <v>0</v>
-      </c>
-      <c r="M13" s="12">
-        <v>0</v>
-      </c>
-      <c r="N13" s="12">
-        <v>0</v>
-      </c>
-      <c r="O13" s="12">
-        <v>0</v>
-      </c>
-      <c r="P13" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="12">
-        <v>0</v>
-      </c>
-      <c r="R13" s="12">
-        <v>1</v>
-      </c>
-      <c r="S13" s="12">
-        <v>1</v>
-      </c>
-      <c r="T13" s="12">
-        <v>0</v>
-      </c>
-      <c r="U13" s="26">
-        <v>0</v>
-      </c>
-      <c r="V13" s="12">
-        <v>0</v>
-      </c>
-      <c r="W13" s="12">
+      <c r="J13" s="14">
+        <v>0</v>
+      </c>
+      <c r="K13" s="14">
+        <v>0</v>
+      </c>
+      <c r="L13" s="14">
+        <v>0</v>
+      </c>
+      <c r="M13" s="14">
+        <v>0</v>
+      </c>
+      <c r="N13" s="14">
+        <v>0</v>
+      </c>
+      <c r="O13" s="14">
+        <v>0</v>
+      </c>
+      <c r="P13" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="14">
+        <v>0</v>
+      </c>
+      <c r="R13" s="14">
+        <v>1</v>
+      </c>
+      <c r="S13" s="14">
+        <v>1</v>
+      </c>
+      <c r="T13" s="14">
+        <v>0</v>
+      </c>
+      <c r="U13" s="61">
+        <v>0</v>
+      </c>
+      <c r="V13" s="14">
+        <v>0</v>
+      </c>
+      <c r="W13" s="14">
         <v>0</v>
       </c>
       <c r="X13" s="13"/>
@@ -2950,46 +2951,46 @@
         <v>56</v>
       </c>
       <c r="I14" s="3"/>
-      <c r="J14" s="12">
-        <v>0</v>
-      </c>
-      <c r="K14" s="12">
-        <v>0</v>
-      </c>
-      <c r="L14" s="12">
-        <v>0</v>
-      </c>
-      <c r="M14" s="12">
-        <v>0</v>
-      </c>
-      <c r="N14" s="12">
-        <v>0</v>
-      </c>
-      <c r="O14" s="12">
-        <v>0</v>
-      </c>
-      <c r="P14" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q14" s="12">
-        <v>0</v>
-      </c>
-      <c r="R14" s="12">
-        <v>0</v>
-      </c>
-      <c r="S14" s="12">
-        <v>0</v>
-      </c>
-      <c r="T14" s="12">
-        <v>0</v>
-      </c>
-      <c r="U14" s="12">
-        <v>1</v>
-      </c>
-      <c r="V14" s="12">
-        <v>1</v>
-      </c>
-      <c r="W14" s="12">
+      <c r="J14" s="14">
+        <v>0</v>
+      </c>
+      <c r="K14" s="14">
+        <v>0</v>
+      </c>
+      <c r="L14" s="14">
+        <v>0</v>
+      </c>
+      <c r="M14" s="14">
+        <v>0</v>
+      </c>
+      <c r="N14" s="14">
+        <v>0</v>
+      </c>
+      <c r="O14" s="14">
+        <v>0</v>
+      </c>
+      <c r="P14" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="14">
+        <v>0</v>
+      </c>
+      <c r="R14" s="14">
+        <v>0</v>
+      </c>
+      <c r="S14" s="14">
+        <v>0</v>
+      </c>
+      <c r="T14" s="14">
+        <v>0</v>
+      </c>
+      <c r="U14" s="14">
+        <v>1</v>
+      </c>
+      <c r="V14" s="14">
+        <v>1</v>
+      </c>
+      <c r="W14" s="14">
         <v>0</v>
       </c>
       <c r="X14" s="13"/>
@@ -3158,46 +3159,46 @@
         <v>56</v>
       </c>
       <c r="I15" s="3"/>
-      <c r="J15" s="12">
-        <v>0</v>
-      </c>
-      <c r="K15" s="12">
-        <v>0</v>
-      </c>
-      <c r="L15" s="12">
-        <v>0</v>
-      </c>
-      <c r="M15" s="12">
-        <v>0</v>
-      </c>
-      <c r="N15" s="12">
-        <v>0</v>
-      </c>
-      <c r="O15" s="12">
-        <v>0</v>
-      </c>
-      <c r="P15" s="12">
-        <v>0</v>
-      </c>
-      <c r="Q15" s="12">
-        <v>0</v>
-      </c>
-      <c r="R15" s="12">
-        <v>0</v>
-      </c>
-      <c r="S15" s="12">
-        <v>0</v>
-      </c>
-      <c r="T15" s="12">
-        <v>0</v>
-      </c>
-      <c r="U15" s="12">
-        <v>0</v>
-      </c>
-      <c r="V15" s="12">
-        <v>0</v>
-      </c>
-      <c r="W15" s="12">
+      <c r="J15" s="14">
+        <v>0</v>
+      </c>
+      <c r="K15" s="14">
+        <v>0</v>
+      </c>
+      <c r="L15" s="14">
+        <v>0</v>
+      </c>
+      <c r="M15" s="14">
+        <v>0</v>
+      </c>
+      <c r="N15" s="14">
+        <v>0</v>
+      </c>
+      <c r="O15" s="14">
+        <v>0</v>
+      </c>
+      <c r="P15" s="14">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="14">
+        <v>0</v>
+      </c>
+      <c r="R15" s="14">
+        <v>0</v>
+      </c>
+      <c r="S15" s="14">
+        <v>0</v>
+      </c>
+      <c r="T15" s="14">
+        <v>0</v>
+      </c>
+      <c r="U15" s="14">
+        <v>0</v>
+      </c>
+      <c r="V15" s="14">
+        <v>0</v>
+      </c>
+      <c r="W15" s="14">
         <v>1</v>
       </c>
       <c r="X15" s="13"/>
@@ -3473,46 +3474,46 @@
         <v>56</v>
       </c>
       <c r="I17" s="3"/>
-      <c r="J17" s="14">
-        <v>1</v>
-      </c>
-      <c r="K17" s="14">
-        <v>0</v>
-      </c>
-      <c r="L17" s="14">
-        <v>0</v>
-      </c>
-      <c r="M17" s="14">
-        <v>0</v>
-      </c>
-      <c r="N17" s="14">
-        <v>0</v>
-      </c>
-      <c r="O17" s="14">
-        <v>0</v>
-      </c>
-      <c r="P17" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="14">
-        <v>0</v>
-      </c>
-      <c r="R17" s="14">
-        <v>0</v>
-      </c>
-      <c r="S17" s="14">
-        <v>0</v>
-      </c>
-      <c r="T17" s="14">
-        <v>0</v>
-      </c>
-      <c r="U17" s="14">
-        <v>0</v>
-      </c>
-      <c r="V17" s="14">
-        <v>0</v>
-      </c>
-      <c r="W17" s="14">
+      <c r="J17" s="12">
+        <v>1</v>
+      </c>
+      <c r="K17" s="12">
+        <v>0</v>
+      </c>
+      <c r="L17" s="12">
+        <v>0</v>
+      </c>
+      <c r="M17" s="12">
+        <v>0</v>
+      </c>
+      <c r="N17" s="12">
+        <v>0</v>
+      </c>
+      <c r="O17" s="12">
+        <v>0</v>
+      </c>
+      <c r="P17" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="12">
+        <v>0</v>
+      </c>
+      <c r="R17" s="12">
+        <v>0</v>
+      </c>
+      <c r="S17" s="12">
+        <v>0</v>
+      </c>
+      <c r="T17" s="12">
+        <v>0</v>
+      </c>
+      <c r="U17" s="12">
+        <v>0</v>
+      </c>
+      <c r="V17" s="12">
+        <v>0</v>
+      </c>
+      <c r="W17" s="12">
         <v>0</v>
       </c>
       <c r="X17" s="13"/>
@@ -3632,46 +3633,46 @@
         <v>56</v>
       </c>
       <c r="I18" s="3"/>
-      <c r="J18" s="14">
-        <v>0</v>
-      </c>
-      <c r="K18" s="14">
-        <v>1</v>
-      </c>
-      <c r="L18" s="14">
-        <v>0</v>
-      </c>
-      <c r="M18" s="14">
-        <v>0</v>
-      </c>
-      <c r="N18" s="14">
-        <v>0</v>
-      </c>
-      <c r="O18" s="14">
-        <v>0</v>
-      </c>
-      <c r="P18" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="14">
-        <v>0</v>
-      </c>
-      <c r="R18" s="14">
-        <v>0</v>
-      </c>
-      <c r="S18" s="14">
-        <v>0</v>
-      </c>
-      <c r="T18" s="14">
-        <v>0</v>
-      </c>
-      <c r="U18" s="14">
-        <v>0</v>
-      </c>
-      <c r="V18" s="14">
-        <v>0</v>
-      </c>
-      <c r="W18" s="14">
+      <c r="J18" s="12">
+        <v>0</v>
+      </c>
+      <c r="K18" s="12">
+        <v>1</v>
+      </c>
+      <c r="L18" s="12">
+        <v>0</v>
+      </c>
+      <c r="M18" s="12">
+        <v>0</v>
+      </c>
+      <c r="N18" s="12">
+        <v>0</v>
+      </c>
+      <c r="O18" s="12">
+        <v>0</v>
+      </c>
+      <c r="P18" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="12">
+        <v>0</v>
+      </c>
+      <c r="R18" s="12">
+        <v>0</v>
+      </c>
+      <c r="S18" s="12">
+        <v>0</v>
+      </c>
+      <c r="T18" s="12">
+        <v>0</v>
+      </c>
+      <c r="U18" s="12">
+        <v>0</v>
+      </c>
+      <c r="V18" s="12">
+        <v>0</v>
+      </c>
+      <c r="W18" s="12">
         <v>0</v>
       </c>
       <c r="X18" s="13"/>
@@ -3792,46 +3793,46 @@
         <v>56</v>
       </c>
       <c r="I19" s="3"/>
-      <c r="J19" s="14">
-        <v>0</v>
-      </c>
-      <c r="K19" s="14">
-        <v>0</v>
-      </c>
-      <c r="L19" s="14">
+      <c r="J19" s="12">
+        <v>0</v>
+      </c>
+      <c r="K19" s="12">
+        <v>0</v>
+      </c>
+      <c r="L19" s="12">
         <v>-1</v>
       </c>
-      <c r="M19" s="14">
-        <v>0</v>
-      </c>
-      <c r="N19" s="14">
-        <v>0</v>
-      </c>
-      <c r="O19" s="14">
-        <v>0</v>
-      </c>
-      <c r="P19" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q19" s="14">
-        <v>0</v>
-      </c>
-      <c r="R19" s="14">
-        <v>0</v>
-      </c>
-      <c r="S19" s="14">
-        <v>0</v>
-      </c>
-      <c r="T19" s="14">
-        <v>0</v>
-      </c>
-      <c r="U19" s="14">
-        <v>0</v>
-      </c>
-      <c r="V19" s="14">
-        <v>0</v>
-      </c>
-      <c r="W19" s="14">
+      <c r="M19" s="12">
+        <v>0</v>
+      </c>
+      <c r="N19" s="12">
+        <v>0</v>
+      </c>
+      <c r="O19" s="12">
+        <v>0</v>
+      </c>
+      <c r="P19" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="12">
+        <v>0</v>
+      </c>
+      <c r="R19" s="12">
+        <v>0</v>
+      </c>
+      <c r="S19" s="12">
+        <v>0</v>
+      </c>
+      <c r="T19" s="12">
+        <v>0</v>
+      </c>
+      <c r="U19" s="12">
+        <v>0</v>
+      </c>
+      <c r="V19" s="12">
+        <v>0</v>
+      </c>
+      <c r="W19" s="12">
         <v>0</v>
       </c>
       <c r="X19" s="13"/>
@@ -3943,46 +3944,46 @@
         <v>56</v>
       </c>
       <c r="I20" s="3"/>
-      <c r="J20" s="14">
-        <v>0</v>
-      </c>
-      <c r="K20" s="14">
-        <v>0</v>
-      </c>
-      <c r="L20" s="14">
-        <v>0</v>
-      </c>
-      <c r="M20" s="14">
-        <v>1</v>
-      </c>
-      <c r="N20" s="14">
-        <v>0</v>
-      </c>
-      <c r="O20" s="14">
-        <v>0</v>
-      </c>
-      <c r="P20" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q20" s="14">
-        <v>0</v>
-      </c>
-      <c r="R20" s="14">
-        <v>0</v>
-      </c>
-      <c r="S20" s="14">
-        <v>0</v>
-      </c>
-      <c r="T20" s="14">
-        <v>0</v>
-      </c>
-      <c r="U20" s="14">
-        <v>0</v>
-      </c>
-      <c r="V20" s="14">
-        <v>0</v>
-      </c>
-      <c r="W20" s="14">
+      <c r="J20" s="12">
+        <v>0</v>
+      </c>
+      <c r="K20" s="12">
+        <v>0</v>
+      </c>
+      <c r="L20" s="12">
+        <v>0</v>
+      </c>
+      <c r="M20" s="12">
+        <v>1</v>
+      </c>
+      <c r="N20" s="12">
+        <v>0</v>
+      </c>
+      <c r="O20" s="12">
+        <v>0</v>
+      </c>
+      <c r="P20" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="12">
+        <v>0</v>
+      </c>
+      <c r="R20" s="12">
+        <v>0</v>
+      </c>
+      <c r="S20" s="12">
+        <v>0</v>
+      </c>
+      <c r="T20" s="12">
+        <v>0</v>
+      </c>
+      <c r="U20" s="12">
+        <v>0</v>
+      </c>
+      <c r="V20" s="12">
+        <v>0</v>
+      </c>
+      <c r="W20" s="12">
         <v>0</v>
       </c>
       <c r="X20" s="13"/>
@@ -4094,46 +4095,46 @@
         <v>56</v>
       </c>
       <c r="I21" s="3"/>
-      <c r="J21" s="14">
-        <v>0</v>
-      </c>
-      <c r="K21" s="14">
-        <v>0</v>
-      </c>
-      <c r="L21" s="14">
-        <v>0</v>
-      </c>
-      <c r="M21" s="14">
-        <v>0</v>
-      </c>
-      <c r="N21" s="14">
-        <v>1</v>
-      </c>
-      <c r="O21" s="14">
-        <v>0</v>
-      </c>
-      <c r="P21" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q21" s="14">
-        <v>0</v>
-      </c>
-      <c r="R21" s="14">
-        <v>0</v>
-      </c>
-      <c r="S21" s="14">
-        <v>0</v>
-      </c>
-      <c r="T21" s="14">
-        <v>0</v>
-      </c>
-      <c r="U21" s="14">
-        <v>0</v>
-      </c>
-      <c r="V21" s="14">
-        <v>0</v>
-      </c>
-      <c r="W21" s="14">
+      <c r="J21" s="12">
+        <v>0</v>
+      </c>
+      <c r="K21" s="12">
+        <v>0</v>
+      </c>
+      <c r="L21" s="12">
+        <v>0</v>
+      </c>
+      <c r="M21" s="12">
+        <v>0</v>
+      </c>
+      <c r="N21" s="12">
+        <v>1</v>
+      </c>
+      <c r="O21" s="12">
+        <v>0</v>
+      </c>
+      <c r="P21" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="12">
+        <v>0</v>
+      </c>
+      <c r="R21" s="12">
+        <v>0</v>
+      </c>
+      <c r="S21" s="12">
+        <v>0</v>
+      </c>
+      <c r="T21" s="12">
+        <v>0</v>
+      </c>
+      <c r="U21" s="12">
+        <v>0</v>
+      </c>
+      <c r="V21" s="12">
+        <v>0</v>
+      </c>
+      <c r="W21" s="12">
         <v>0</v>
       </c>
       <c r="X21" s="13"/>
@@ -4238,46 +4239,46 @@
         <v>56</v>
       </c>
       <c r="I22" s="3"/>
-      <c r="J22" s="14">
-        <v>0</v>
-      </c>
-      <c r="K22" s="14">
-        <v>0</v>
-      </c>
-      <c r="L22" s="14">
-        <v>0</v>
-      </c>
-      <c r="M22" s="14">
-        <v>0</v>
-      </c>
-      <c r="N22" s="14">
-        <v>1</v>
-      </c>
-      <c r="O22" s="14">
-        <v>0</v>
-      </c>
-      <c r="P22" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q22" s="14">
-        <v>0</v>
-      </c>
-      <c r="R22" s="14">
-        <v>0</v>
-      </c>
-      <c r="S22" s="14">
-        <v>0</v>
-      </c>
-      <c r="T22" s="14">
-        <v>0</v>
-      </c>
-      <c r="U22" s="14">
-        <v>0</v>
-      </c>
-      <c r="V22" s="14">
-        <v>0</v>
-      </c>
-      <c r="W22" s="14">
+      <c r="J22" s="12">
+        <v>0</v>
+      </c>
+      <c r="K22" s="12">
+        <v>0</v>
+      </c>
+      <c r="L22" s="12">
+        <v>0</v>
+      </c>
+      <c r="M22" s="12">
+        <v>0</v>
+      </c>
+      <c r="N22" s="12">
+        <v>1</v>
+      </c>
+      <c r="O22" s="12">
+        <v>0</v>
+      </c>
+      <c r="P22" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="12">
+        <v>0</v>
+      </c>
+      <c r="R22" s="12">
+        <v>0</v>
+      </c>
+      <c r="S22" s="12">
+        <v>0</v>
+      </c>
+      <c r="T22" s="12">
+        <v>0</v>
+      </c>
+      <c r="U22" s="12">
+        <v>0</v>
+      </c>
+      <c r="V22" s="12">
+        <v>0</v>
+      </c>
+      <c r="W22" s="12">
         <v>0</v>
       </c>
       <c r="X22" s="13"/>
@@ -4380,46 +4381,46 @@
         <v>56</v>
       </c>
       <c r="I23" s="3"/>
-      <c r="J23" s="14">
-        <v>0</v>
-      </c>
-      <c r="K23" s="14">
-        <v>0</v>
-      </c>
-      <c r="L23" s="14">
-        <v>0</v>
-      </c>
-      <c r="M23" s="14">
-        <v>0</v>
-      </c>
-      <c r="N23" s="14">
-        <v>0</v>
-      </c>
-      <c r="O23" s="14">
-        <v>1</v>
-      </c>
-      <c r="P23" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q23" s="14">
-        <v>0</v>
-      </c>
-      <c r="R23" s="14">
-        <v>0</v>
-      </c>
-      <c r="S23" s="14">
-        <v>0</v>
-      </c>
-      <c r="T23" s="14">
-        <v>0</v>
-      </c>
-      <c r="U23" s="14">
-        <v>0</v>
-      </c>
-      <c r="V23" s="14">
-        <v>0</v>
-      </c>
-      <c r="W23" s="14">
+      <c r="J23" s="12">
+        <v>0</v>
+      </c>
+      <c r="K23" s="12">
+        <v>0</v>
+      </c>
+      <c r="L23" s="12">
+        <v>0</v>
+      </c>
+      <c r="M23" s="12">
+        <v>0</v>
+      </c>
+      <c r="N23" s="12">
+        <v>0</v>
+      </c>
+      <c r="O23" s="12">
+        <v>1</v>
+      </c>
+      <c r="P23" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="12">
+        <v>0</v>
+      </c>
+      <c r="R23" s="12">
+        <v>0</v>
+      </c>
+      <c r="S23" s="12">
+        <v>0</v>
+      </c>
+      <c r="T23" s="12">
+        <v>0</v>
+      </c>
+      <c r="U23" s="12">
+        <v>0</v>
+      </c>
+      <c r="V23" s="12">
+        <v>0</v>
+      </c>
+      <c r="W23" s="12">
         <v>0</v>
       </c>
       <c r="X23" s="13"/>
@@ -4530,46 +4531,46 @@
         <v>56</v>
       </c>
       <c r="I24" s="3"/>
-      <c r="J24" s="14">
-        <v>0</v>
-      </c>
-      <c r="K24" s="14">
-        <v>0</v>
-      </c>
-      <c r="L24" s="14">
-        <v>0</v>
-      </c>
-      <c r="M24" s="14">
-        <v>0</v>
-      </c>
-      <c r="N24" s="14">
-        <v>0</v>
-      </c>
-      <c r="O24" s="14">
-        <v>0</v>
-      </c>
-      <c r="P24" s="14">
-        <v>1</v>
-      </c>
-      <c r="Q24" s="14">
-        <v>0</v>
-      </c>
-      <c r="R24" s="14">
-        <v>0</v>
-      </c>
-      <c r="S24" s="14">
-        <v>0</v>
-      </c>
-      <c r="T24" s="14">
-        <v>0</v>
-      </c>
-      <c r="U24" s="14">
-        <v>0</v>
-      </c>
-      <c r="V24" s="14">
-        <v>0</v>
-      </c>
-      <c r="W24" s="14">
+      <c r="J24" s="12">
+        <v>0</v>
+      </c>
+      <c r="K24" s="12">
+        <v>0</v>
+      </c>
+      <c r="L24" s="12">
+        <v>0</v>
+      </c>
+      <c r="M24" s="12">
+        <v>0</v>
+      </c>
+      <c r="N24" s="12">
+        <v>0</v>
+      </c>
+      <c r="O24" s="12">
+        <v>0</v>
+      </c>
+      <c r="P24" s="12">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="12">
+        <v>0</v>
+      </c>
+      <c r="R24" s="12">
+        <v>0</v>
+      </c>
+      <c r="S24" s="12">
+        <v>0</v>
+      </c>
+      <c r="T24" s="12">
+        <v>0</v>
+      </c>
+      <c r="U24" s="12">
+        <v>0</v>
+      </c>
+      <c r="V24" s="12">
+        <v>0</v>
+      </c>
+      <c r="W24" s="12">
         <v>0</v>
       </c>
       <c r="X24" s="13"/>
@@ -4680,46 +4681,46 @@
         <v>56</v>
       </c>
       <c r="I25" s="3"/>
-      <c r="J25" s="14">
-        <v>0</v>
-      </c>
-      <c r="K25" s="14">
-        <v>0</v>
-      </c>
-      <c r="L25" s="14">
-        <v>0</v>
-      </c>
-      <c r="M25" s="14">
-        <v>0</v>
-      </c>
-      <c r="N25" s="14">
-        <v>0</v>
-      </c>
-      <c r="O25" s="14">
-        <v>0</v>
-      </c>
-      <c r="P25" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="14">
-        <v>1</v>
-      </c>
-      <c r="R25" s="14">
-        <v>0</v>
-      </c>
-      <c r="S25" s="14">
-        <v>0</v>
-      </c>
-      <c r="T25" s="14">
-        <v>0</v>
-      </c>
-      <c r="U25" s="14">
-        <v>0</v>
-      </c>
-      <c r="V25" s="14">
-        <v>0</v>
-      </c>
-      <c r="W25" s="14">
+      <c r="J25" s="12">
+        <v>0</v>
+      </c>
+      <c r="K25" s="12">
+        <v>0</v>
+      </c>
+      <c r="L25" s="12">
+        <v>0</v>
+      </c>
+      <c r="M25" s="12">
+        <v>0</v>
+      </c>
+      <c r="N25" s="12">
+        <v>0</v>
+      </c>
+      <c r="O25" s="12">
+        <v>0</v>
+      </c>
+      <c r="P25" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="12">
+        <v>1</v>
+      </c>
+      <c r="R25" s="12">
+        <v>0</v>
+      </c>
+      <c r="S25" s="12">
+        <v>0</v>
+      </c>
+      <c r="T25" s="12">
+        <v>0</v>
+      </c>
+      <c r="U25" s="12">
+        <v>0</v>
+      </c>
+      <c r="V25" s="12">
+        <v>0</v>
+      </c>
+      <c r="W25" s="12">
         <v>0</v>
       </c>
       <c r="X25" s="13"/>
@@ -4830,46 +4831,46 @@
         <v>56</v>
       </c>
       <c r="I26" s="3"/>
-      <c r="J26" s="14">
-        <v>0</v>
-      </c>
-      <c r="K26" s="14">
-        <v>0</v>
-      </c>
-      <c r="L26" s="14">
-        <v>0</v>
-      </c>
-      <c r="M26" s="14">
-        <v>0</v>
-      </c>
-      <c r="N26" s="14">
-        <v>0</v>
-      </c>
-      <c r="O26" s="14">
-        <v>0</v>
-      </c>
-      <c r="P26" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q26" s="14">
-        <v>0</v>
-      </c>
-      <c r="R26" s="14">
-        <v>0</v>
-      </c>
-      <c r="S26" s="14">
-        <v>0</v>
-      </c>
-      <c r="T26" s="14">
-        <v>0</v>
-      </c>
-      <c r="U26" s="14">
-        <v>0</v>
-      </c>
-      <c r="V26" s="14">
-        <v>0</v>
-      </c>
-      <c r="W26" s="14">
+      <c r="J26" s="12">
+        <v>0</v>
+      </c>
+      <c r="K26" s="12">
+        <v>0</v>
+      </c>
+      <c r="L26" s="12">
+        <v>0</v>
+      </c>
+      <c r="M26" s="12">
+        <v>0</v>
+      </c>
+      <c r="N26" s="12">
+        <v>0</v>
+      </c>
+      <c r="O26" s="12">
+        <v>0</v>
+      </c>
+      <c r="P26" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="12">
+        <v>0</v>
+      </c>
+      <c r="R26" s="12">
+        <v>0</v>
+      </c>
+      <c r="S26" s="12">
+        <v>0</v>
+      </c>
+      <c r="T26" s="12">
+        <v>0</v>
+      </c>
+      <c r="U26" s="12">
+        <v>0</v>
+      </c>
+      <c r="V26" s="12">
+        <v>0</v>
+      </c>
+      <c r="W26" s="12">
         <v>0</v>
       </c>
       <c r="X26" s="13"/>
@@ -4983,46 +4984,46 @@
         <v>56</v>
       </c>
       <c r="I27" s="3"/>
-      <c r="J27" s="14">
-        <v>0</v>
-      </c>
-      <c r="K27" s="14">
-        <v>0</v>
-      </c>
-      <c r="L27" s="14">
-        <v>0</v>
-      </c>
-      <c r="M27" s="14">
-        <v>0</v>
-      </c>
-      <c r="N27" s="14">
-        <v>0</v>
-      </c>
-      <c r="O27" s="14">
-        <v>0</v>
-      </c>
-      <c r="P27" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q27" s="14">
-        <v>0</v>
-      </c>
-      <c r="R27" s="14">
-        <v>1</v>
-      </c>
-      <c r="S27" s="14">
-        <v>0</v>
-      </c>
-      <c r="T27" s="14">
-        <v>0</v>
-      </c>
-      <c r="U27" s="14">
-        <v>0</v>
-      </c>
-      <c r="V27" s="14">
-        <v>0</v>
-      </c>
-      <c r="W27" s="14">
+      <c r="J27" s="12">
+        <v>0</v>
+      </c>
+      <c r="K27" s="12">
+        <v>0</v>
+      </c>
+      <c r="L27" s="12">
+        <v>0</v>
+      </c>
+      <c r="M27" s="12">
+        <v>0</v>
+      </c>
+      <c r="N27" s="12">
+        <v>0</v>
+      </c>
+      <c r="O27" s="12">
+        <v>0</v>
+      </c>
+      <c r="P27" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="12">
+        <v>0</v>
+      </c>
+      <c r="R27" s="12">
+        <v>1</v>
+      </c>
+      <c r="S27" s="12">
+        <v>0</v>
+      </c>
+      <c r="T27" s="12">
+        <v>0</v>
+      </c>
+      <c r="U27" s="12">
+        <v>0</v>
+      </c>
+      <c r="V27" s="12">
+        <v>0</v>
+      </c>
+      <c r="W27" s="12">
         <v>0</v>
       </c>
       <c r="X27" s="13"/>
@@ -5155,46 +5156,46 @@
         <v>56</v>
       </c>
       <c r="I28" s="3"/>
-      <c r="J28" s="14">
-        <v>0</v>
-      </c>
-      <c r="K28" s="14">
-        <v>0</v>
-      </c>
-      <c r="L28" s="14">
-        <v>0</v>
-      </c>
-      <c r="M28" s="14">
-        <v>0</v>
-      </c>
-      <c r="N28" s="14">
-        <v>0</v>
-      </c>
-      <c r="O28" s="14">
-        <v>0</v>
-      </c>
-      <c r="P28" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="14">
-        <v>0</v>
-      </c>
-      <c r="R28" s="14">
-        <v>0</v>
-      </c>
-      <c r="S28" s="14">
-        <v>1</v>
-      </c>
-      <c r="T28" s="14">
-        <v>0</v>
-      </c>
-      <c r="U28" s="14">
-        <v>0</v>
-      </c>
-      <c r="V28" s="14">
-        <v>0</v>
-      </c>
-      <c r="W28" s="14">
+      <c r="J28" s="12">
+        <v>0</v>
+      </c>
+      <c r="K28" s="12">
+        <v>0</v>
+      </c>
+      <c r="L28" s="12">
+        <v>0</v>
+      </c>
+      <c r="M28" s="12">
+        <v>0</v>
+      </c>
+      <c r="N28" s="12">
+        <v>0</v>
+      </c>
+      <c r="O28" s="12">
+        <v>0</v>
+      </c>
+      <c r="P28" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="12">
+        <v>0</v>
+      </c>
+      <c r="R28" s="12">
+        <v>0</v>
+      </c>
+      <c r="S28" s="12">
+        <v>1</v>
+      </c>
+      <c r="T28" s="12">
+        <v>0</v>
+      </c>
+      <c r="U28" s="12">
+        <v>0</v>
+      </c>
+      <c r="V28" s="12">
+        <v>0</v>
+      </c>
+      <c r="W28" s="12">
         <v>0</v>
       </c>
       <c r="X28" s="13"/>
@@ -5314,46 +5315,46 @@
         <v>56</v>
       </c>
       <c r="I29" s="3"/>
-      <c r="J29" s="14">
-        <v>0</v>
-      </c>
-      <c r="K29" s="14">
-        <v>0</v>
-      </c>
-      <c r="L29" s="14">
-        <v>0</v>
-      </c>
-      <c r="M29" s="14">
-        <v>0</v>
-      </c>
-      <c r="N29" s="14">
-        <v>0</v>
-      </c>
-      <c r="O29" s="14">
-        <v>0</v>
-      </c>
-      <c r="P29" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="14">
-        <v>0</v>
-      </c>
-      <c r="R29" s="14">
-        <v>0</v>
-      </c>
-      <c r="S29" s="14">
-        <v>0</v>
-      </c>
-      <c r="T29" s="14">
-        <v>1</v>
-      </c>
-      <c r="U29" s="14">
-        <v>0</v>
-      </c>
-      <c r="V29" s="14">
-        <v>0</v>
-      </c>
-      <c r="W29" s="14">
+      <c r="J29" s="12">
+        <v>0</v>
+      </c>
+      <c r="K29" s="12">
+        <v>0</v>
+      </c>
+      <c r="L29" s="12">
+        <v>0</v>
+      </c>
+      <c r="M29" s="12">
+        <v>0</v>
+      </c>
+      <c r="N29" s="12">
+        <v>0</v>
+      </c>
+      <c r="O29" s="12">
+        <v>0</v>
+      </c>
+      <c r="P29" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="12">
+        <v>0</v>
+      </c>
+      <c r="R29" s="12">
+        <v>0</v>
+      </c>
+      <c r="S29" s="12">
+        <v>0</v>
+      </c>
+      <c r="T29" s="12">
+        <v>1</v>
+      </c>
+      <c r="U29" s="12">
+        <v>0</v>
+      </c>
+      <c r="V29" s="12">
+        <v>0</v>
+      </c>
+      <c r="W29" s="12">
         <v>0</v>
       </c>
       <c r="X29" s="13"/>
@@ -5447,46 +5448,46 @@
         <v>56</v>
       </c>
       <c r="I30" s="3"/>
-      <c r="J30" s="14">
-        <v>0</v>
-      </c>
-      <c r="K30" s="14">
-        <v>0</v>
-      </c>
-      <c r="L30" s="14">
-        <v>0</v>
-      </c>
-      <c r="M30" s="14">
-        <v>0</v>
-      </c>
-      <c r="N30" s="14">
-        <v>0</v>
-      </c>
-      <c r="O30" s="14">
-        <v>0</v>
-      </c>
-      <c r="P30" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="14">
-        <v>0</v>
-      </c>
-      <c r="R30" s="14">
-        <v>0</v>
-      </c>
-      <c r="S30" s="14">
-        <v>0</v>
-      </c>
-      <c r="T30" s="14">
-        <v>0</v>
-      </c>
-      <c r="U30" s="14">
-        <v>1</v>
-      </c>
-      <c r="V30" s="14">
-        <v>0</v>
-      </c>
-      <c r="W30" s="14">
+      <c r="J30" s="12">
+        <v>0</v>
+      </c>
+      <c r="K30" s="12">
+        <v>0</v>
+      </c>
+      <c r="L30" s="12">
+        <v>0</v>
+      </c>
+      <c r="M30" s="12">
+        <v>0</v>
+      </c>
+      <c r="N30" s="12">
+        <v>0</v>
+      </c>
+      <c r="O30" s="12">
+        <v>0</v>
+      </c>
+      <c r="P30" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="12">
+        <v>0</v>
+      </c>
+      <c r="R30" s="12">
+        <v>0</v>
+      </c>
+      <c r="S30" s="12">
+        <v>0</v>
+      </c>
+      <c r="T30" s="12">
+        <v>0</v>
+      </c>
+      <c r="U30" s="12">
+        <v>1</v>
+      </c>
+      <c r="V30" s="12">
+        <v>0</v>
+      </c>
+      <c r="W30" s="12">
         <v>0</v>
       </c>
       <c r="X30" s="13"/>
@@ -5594,46 +5595,46 @@
         <v>56</v>
       </c>
       <c r="I31" s="3"/>
-      <c r="J31" s="14">
-        <v>0</v>
-      </c>
-      <c r="K31" s="14">
-        <v>0</v>
-      </c>
-      <c r="L31" s="14">
-        <v>0</v>
-      </c>
-      <c r="M31" s="14">
-        <v>0</v>
-      </c>
-      <c r="N31" s="14">
-        <v>0</v>
-      </c>
-      <c r="O31" s="14">
-        <v>0</v>
-      </c>
-      <c r="P31" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q31" s="14">
-        <v>0</v>
-      </c>
-      <c r="R31" s="14">
-        <v>0</v>
-      </c>
-      <c r="S31" s="14">
-        <v>0</v>
-      </c>
-      <c r="T31" s="14">
-        <v>0</v>
-      </c>
-      <c r="U31" s="14">
-        <v>0</v>
-      </c>
-      <c r="V31" s="14">
-        <v>1</v>
-      </c>
-      <c r="W31" s="14">
+      <c r="J31" s="12">
+        <v>0</v>
+      </c>
+      <c r="K31" s="12">
+        <v>0</v>
+      </c>
+      <c r="L31" s="12">
+        <v>0</v>
+      </c>
+      <c r="M31" s="12">
+        <v>0</v>
+      </c>
+      <c r="N31" s="12">
+        <v>0</v>
+      </c>
+      <c r="O31" s="12">
+        <v>0</v>
+      </c>
+      <c r="P31" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="12">
+        <v>0</v>
+      </c>
+      <c r="R31" s="12">
+        <v>0</v>
+      </c>
+      <c r="S31" s="12">
+        <v>0</v>
+      </c>
+      <c r="T31" s="12">
+        <v>0</v>
+      </c>
+      <c r="U31" s="12">
+        <v>0</v>
+      </c>
+      <c r="V31" s="12">
+        <v>1</v>
+      </c>
+      <c r="W31" s="12">
         <v>0</v>
       </c>
       <c r="X31" s="13"/>
@@ -5756,46 +5757,46 @@
         <v>56</v>
       </c>
       <c r="I32" s="3"/>
-      <c r="J32" s="14">
-        <v>0</v>
-      </c>
-      <c r="K32" s="14">
-        <v>0</v>
-      </c>
-      <c r="L32" s="14">
-        <v>0</v>
-      </c>
-      <c r="M32" s="14">
-        <v>0</v>
-      </c>
-      <c r="N32" s="14">
-        <v>0</v>
-      </c>
-      <c r="O32" s="14">
-        <v>0</v>
-      </c>
-      <c r="P32" s="14">
-        <v>0</v>
-      </c>
-      <c r="Q32" s="14">
-        <v>0</v>
-      </c>
-      <c r="R32" s="14">
-        <v>0</v>
-      </c>
-      <c r="S32" s="14">
-        <v>0</v>
-      </c>
-      <c r="T32" s="14">
-        <v>0</v>
-      </c>
-      <c r="U32" s="14">
-        <v>0</v>
-      </c>
-      <c r="V32" s="14">
-        <v>0</v>
-      </c>
-      <c r="W32" s="14">
+      <c r="J32" s="12">
+        <v>0</v>
+      </c>
+      <c r="K32" s="12">
+        <v>0</v>
+      </c>
+      <c r="L32" s="12">
+        <v>0</v>
+      </c>
+      <c r="M32" s="12">
+        <v>0</v>
+      </c>
+      <c r="N32" s="12">
+        <v>0</v>
+      </c>
+      <c r="O32" s="12">
+        <v>0</v>
+      </c>
+      <c r="P32" s="12">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="12">
+        <v>0</v>
+      </c>
+      <c r="R32" s="12">
+        <v>0</v>
+      </c>
+      <c r="S32" s="12">
+        <v>0</v>
+      </c>
+      <c r="T32" s="12">
+        <v>0</v>
+      </c>
+      <c r="U32" s="12">
+        <v>0</v>
+      </c>
+      <c r="V32" s="12">
+        <v>0</v>
+      </c>
+      <c r="W32" s="12">
         <v>1</v>
       </c>
       <c r="X32" s="13"/>

</xml_diff>